<commit_message>
maj dossier et interface combat
</commit_message>
<xml_diff>
--- a/data/terrain.xlsx
+++ b/data/terrain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hghos\Documents\Perso_APH\travail\ENSG-Géomatique\POO\Projet\COUDERC-HOSTEIN-LANCHA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465871E7-068B-479B-AAA4-E79A85D13B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F6C599-FC6B-4046-B34F-7EB76DD4C0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF96B166-02CE-447C-B2BB-029EF137380B}"/>
   </bookViews>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F280D1FC-DF26-40C3-B7BD-474909A5227D}">
   <dimension ref="A1:DG108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK93" activeCellId="7" sqref="BU85:BV87 BO101:BP101 BE101:BF101 AZ101 AS99:AU100 AL98:AM98 AH96:AH97 AI92:AK93"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CN68" sqref="CL68:CN68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18720,19 +18720,19 @@
         <v>5</v>
       </c>
       <c r="BK55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BP55">
         <v>5</v>
@@ -19055,19 +19055,19 @@
         <v>5</v>
       </c>
       <c r="BK56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BP56">
         <v>5</v>
@@ -19390,19 +19390,19 @@
         <v>5</v>
       </c>
       <c r="BK57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BP57">
         <v>5</v>
@@ -19716,25 +19716,25 @@
         <v>5</v>
       </c>
       <c r="BH58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BI58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BJ58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BK58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO58">
         <v>5</v>
@@ -20051,25 +20051,25 @@
         <v>5</v>
       </c>
       <c r="BH59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BI59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BJ59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BK59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO59">
         <v>5</v>
@@ -20081,19 +20081,19 @@
         <v>5</v>
       </c>
       <c r="BR59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BS59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BT59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BU59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BV59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BW59">
         <v>5</v>
@@ -20392,19 +20392,19 @@
         <v>5</v>
       </c>
       <c r="BJ60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BK60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BL60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BM60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BN60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BO60">
         <v>5</v>
@@ -20416,19 +20416,19 @@
         <v>5</v>
       </c>
       <c r="BR60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BS60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BT60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BU60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BV60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BW60">
         <v>5</v>
@@ -20751,19 +20751,19 @@
         <v>5</v>
       </c>
       <c r="BR61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BS61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BT61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BU61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BV61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BW61">
         <v>5</v>
@@ -20924,22 +20924,22 @@
         <v>1</v>
       </c>
       <c r="P62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R62">
         <v>1</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V62">
         <v>1</v>
@@ -21086,19 +21086,19 @@
         <v>5</v>
       </c>
       <c r="BR62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BS62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BT62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BU62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BV62">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BW62">
         <v>5</v>
@@ -23135,34 +23135,34 @@
         <v>5</v>
       </c>
       <c r="CE68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CF68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CG68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CH68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CI68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CJ68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CK68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CL68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CM68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CN68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CO68">
         <v>5</v>
@@ -23485,10 +23485,10 @@
         <v>5</v>
       </c>
       <c r="CJ69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CK69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CL69">
         <v>5</v>
@@ -23820,10 +23820,10 @@
         <v>5</v>
       </c>
       <c r="CJ70">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CK70">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CL70">
         <v>5</v>
@@ -24128,37 +24128,37 @@
         <v>3</v>
       </c>
       <c r="CA71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CD71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CE71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CF71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CG71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CH71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CI71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CJ71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CK71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CL71">
         <v>5</v>
@@ -24463,37 +24463,37 @@
         <v>5</v>
       </c>
       <c r="CA72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CD72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CE72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CF72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CG72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CH72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CI72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CJ72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CK72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CL72">
         <v>5</v>
@@ -24798,10 +24798,10 @@
         <v>5</v>
       </c>
       <c r="CA73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC73">
         <v>5</v>
@@ -25133,10 +25133,10 @@
         <v>5</v>
       </c>
       <c r="CA74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC74">
         <v>5</v>
@@ -25432,46 +25432,46 @@
         <v>4</v>
       </c>
       <c r="BO75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BP75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BQ75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BR75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BS75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BT75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BU75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BV75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BW75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BX75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BY75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZ75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CA75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC75">
         <v>5</v>
@@ -25767,46 +25767,46 @@
         <v>4</v>
       </c>
       <c r="BO76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BP76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BQ76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BR76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BS76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BT76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BU76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BV76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BW76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BX76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BY76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZ76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CA76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC76">
         <v>5</v>
@@ -26102,10 +26102,10 @@
         <v>4</v>
       </c>
       <c r="BO77">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BP77">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BQ77">
         <v>5</v>
@@ -26138,10 +26138,10 @@
         <v>5</v>
       </c>
       <c r="CA77">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB77">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC77">
         <v>5</v>
@@ -26473,10 +26473,10 @@
         <v>5</v>
       </c>
       <c r="CA78">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB78">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC78">
         <v>5</v>
@@ -26808,10 +26808,10 @@
         <v>5</v>
       </c>
       <c r="CA79">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB79">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC79">
         <v>5</v>
@@ -27107,7 +27107,7 @@
         <v>4</v>
       </c>
       <c r="BO80">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BP80">
         <v>5</v>
@@ -27143,10 +27143,10 @@
         <v>5</v>
       </c>
       <c r="CA80">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB80">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC80">
         <v>5</v>
@@ -27442,7 +27442,7 @@
         <v>4</v>
       </c>
       <c r="BO81">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BP81">
         <v>5</v>
@@ -27478,10 +27478,10 @@
         <v>5</v>
       </c>
       <c r="CA81">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB81">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC81">
         <v>5</v>
@@ -27621,34 +27621,34 @@
         <v>5</v>
       </c>
       <c r="O82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y82">
         <v>4</v>
@@ -27813,10 +27813,10 @@
         <v>5</v>
       </c>
       <c r="CA82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC82">
         <v>5</v>
@@ -27956,34 +27956,34 @@
         <v>5</v>
       </c>
       <c r="O83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y83">
         <v>4</v>
@@ -28148,10 +28148,10 @@
         <v>5</v>
       </c>
       <c r="CA83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC83">
         <v>5</v>
@@ -28291,10 +28291,10 @@
         <v>5</v>
       </c>
       <c r="O84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q84">
         <v>5</v>
@@ -28483,10 +28483,10 @@
         <v>5</v>
       </c>
       <c r="CA84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC84">
         <v>5</v>
@@ -28626,31 +28626,31 @@
         <v>5</v>
       </c>
       <c r="O85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q85">
         <v>5</v>
       </c>
       <c r="R85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S85">
         <v>5</v>
       </c>
       <c r="T85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X85">
         <v>5</v>
@@ -28818,10 +28818,10 @@
         <v>5</v>
       </c>
       <c r="CA85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC85">
         <v>5</v>
@@ -28961,16 +28961,16 @@
         <v>5</v>
       </c>
       <c r="O86">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P86">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q86">
         <v>5</v>
       </c>
       <c r="R86">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S86">
         <v>5</v>
@@ -28985,7 +28985,7 @@
         <v>5</v>
       </c>
       <c r="W86">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X86">
         <v>5</v>
@@ -29153,10 +29153,10 @@
         <v>5</v>
       </c>
       <c r="CA86">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB86">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC86">
         <v>5</v>
@@ -29296,16 +29296,16 @@
         <v>5</v>
       </c>
       <c r="O87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q87">
         <v>5</v>
       </c>
       <c r="R87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S87">
         <v>5</v>
@@ -29320,7 +29320,7 @@
         <v>5</v>
       </c>
       <c r="W87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X87">
         <v>5</v>
@@ -29488,10 +29488,10 @@
         <v>5</v>
       </c>
       <c r="CA87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC87">
         <v>5</v>
@@ -29631,31 +29631,31 @@
         <v>5</v>
       </c>
       <c r="O88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q88">
         <v>5</v>
       </c>
       <c r="R88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X88">
         <v>5</v>
@@ -29823,10 +29823,10 @@
         <v>5</v>
       </c>
       <c r="CA88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC88">
         <v>5</v>
@@ -29966,10 +29966,10 @@
         <v>5</v>
       </c>
       <c r="O89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q89">
         <v>5</v>
@@ -30158,10 +30158,10 @@
         <v>5</v>
       </c>
       <c r="CA89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC89">
         <v>5</v>
@@ -30301,34 +30301,34 @@
         <v>5</v>
       </c>
       <c r="O90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y90">
         <v>4</v>
@@ -30457,7 +30457,7 @@
         <v>4</v>
       </c>
       <c r="BO90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BP90">
         <v>5</v>
@@ -30493,16 +30493,16 @@
         <v>5</v>
       </c>
       <c r="CA90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CD90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CE90">
         <v>5</v>
@@ -30636,34 +30636,34 @@
         <v>5</v>
       </c>
       <c r="O91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y91">
         <v>4</v>
@@ -30792,25 +30792,25 @@
         <v>4</v>
       </c>
       <c r="BO91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BP91">
         <v>5</v>
       </c>
       <c r="BQ91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BR91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BS91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BT91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BU91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BV91">
         <v>5</v>
@@ -30828,16 +30828,16 @@
         <v>5</v>
       </c>
       <c r="CA91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CB91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CC91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CD91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CE91">
         <v>5</v>

</xml_diff>